<commit_message>
added support for IKE Gateways
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudarshanv/Documents/Projects/panospython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E883DC6D-84D6-A749-9765-F72C71A21E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EDA58A-CE9A-FD4D-9F11-75D59D895E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68800" yWindow="7800" windowWidth="33600" windowHeight="21000" firstSheet="3" activeTab="15" xr2:uid="{D24069A8-A644-D445-BA17-ADF18F8BF45D}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="27100" firstSheet="5" activeTab="17" xr2:uid="{D24069A8-A644-D445-BA17-ADF18F8BF45D}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,11 @@
     <sheet name="bgp_peer_groups" sheetId="14" r:id="rId14"/>
     <sheet name="bgp_peers" sheetId="15" r:id="rId15"/>
     <sheet name="ike_crypto_profile" sheetId="16" r:id="rId16"/>
+    <sheet name="ike_gateway" sheetId="17" r:id="rId17"/>
+    <sheet name="ipsec_crypto_profile" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9030" uniqueCount="2002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9420" uniqueCount="2107">
   <si>
     <t>template_name</t>
   </si>
@@ -6055,6 +6058,321 @@
   </si>
   <si>
     <t>Verizon_IKE</t>
+  </si>
+  <si>
+    <t>local_ip_address</t>
+  </si>
+  <si>
+    <t>local_id_type</t>
+  </si>
+  <si>
+    <t>ipaddr</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>local_id_value</t>
+  </si>
+  <si>
+    <t>peer_id_type</t>
+  </si>
+  <si>
+    <t>peer_ip_value</t>
+  </si>
+  <si>
+    <t>ikev2_crypto_profile</t>
+  </si>
+  <si>
+    <t>dead_peer_detection_interval</t>
+  </si>
+  <si>
+    <t>dead_peer_detection_retry</t>
+  </si>
+  <si>
+    <t>A-CDM_Primary</t>
+  </si>
+  <si>
+    <t>A-CDM_Secondary</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_Gateway</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_GATEWAY_1</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_GATEWAY_2</t>
+  </si>
+  <si>
+    <t>ADVAM_TEST_Gateway</t>
+  </si>
+  <si>
+    <t>ADVAM_TEST_Gateway_1</t>
+  </si>
+  <si>
+    <t>ADVAM_TEST_Gateway_2</t>
+  </si>
+  <si>
+    <t>AEROCARE_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>AZURE_MEL_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>AZURE_SYD_IKE_GATEWAY</t>
+  </si>
+  <si>
+    <t>BoM_1_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>BoM_2_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>CROSSCOM_ORION_Gateway</t>
+  </si>
+  <si>
+    <t>ESRI_EGIS_GATEWAY_1</t>
+  </si>
+  <si>
+    <t>ESRI_EGIS_GATEWAY_2</t>
+  </si>
+  <si>
+    <t>ETHAN_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>GENTRACK_Gateway</t>
+  </si>
+  <si>
+    <t>IKE51-LAUNCESTON-IKEv1</t>
+  </si>
+  <si>
+    <t>JETSTAR_JINTERNET_Gateway</t>
+  </si>
+  <si>
+    <t>Logicalis_BaaS</t>
+  </si>
+  <si>
+    <t>SENSOR_DYNAMIC_Gateway</t>
+  </si>
+  <si>
+    <t>Verizon_IKE_Gateway</t>
+  </si>
+  <si>
+    <t>ikev1</t>
+  </si>
+  <si>
+    <t>ikev2-preferred</t>
+  </si>
+  <si>
+    <t>183.177.120.59</t>
+  </si>
+  <si>
+    <t>183.177.120.60</t>
+  </si>
+  <si>
+    <t>183.177.122.117</t>
+  </si>
+  <si>
+    <t>183.177.122.119</t>
+  </si>
+  <si>
+    <t>183.177.122.106</t>
+  </si>
+  <si>
+    <t>183.177.120.55</t>
+  </si>
+  <si>
+    <t>183.177.120.56</t>
+  </si>
+  <si>
+    <t>183.177.123.12</t>
+  </si>
+  <si>
+    <t>183.177.123.13</t>
+  </si>
+  <si>
+    <t>183.177.122.147</t>
+  </si>
+  <si>
+    <t>183.177.123.16</t>
+  </si>
+  <si>
+    <t>183.177.122.47</t>
+  </si>
+  <si>
+    <t>183.177.123.14</t>
+  </si>
+  <si>
+    <t>183.177.120.50</t>
+  </si>
+  <si>
+    <t>183.177.122.83</t>
+  </si>
+  <si>
+    <t>183.177.120.52</t>
+  </si>
+  <si>
+    <t>183.177.123.15</t>
+  </si>
+  <si>
+    <t>183.177.122.65</t>
+  </si>
+  <si>
+    <t>183.177.120.53</t>
+  </si>
+  <si>
+    <t>13.237.189.57</t>
+  </si>
+  <si>
+    <t>54.79.95.179</t>
+  </si>
+  <si>
+    <t>13.236.107.141</t>
+  </si>
+  <si>
+    <t>13.239.164.64</t>
+  </si>
+  <si>
+    <t>54.153.157.17</t>
+  </si>
+  <si>
+    <t>34.242.163.246</t>
+  </si>
+  <si>
+    <t>13.238.73.61</t>
+  </si>
+  <si>
+    <t>52.62.148.121</t>
+  </si>
+  <si>
+    <t>180.214.64.32</t>
+  </si>
+  <si>
+    <t>52.255.47.234</t>
+  </si>
+  <si>
+    <t>20.188.238.245</t>
+  </si>
+  <si>
+    <t>134.178.63.125</t>
+  </si>
+  <si>
+    <t>134.178.253.35</t>
+  </si>
+  <si>
+    <t>202.182.144.6</t>
+  </si>
+  <si>
+    <t>13.210.57.97</t>
+  </si>
+  <si>
+    <t>13.210.190.144</t>
+  </si>
+  <si>
+    <t>103.9.63.145</t>
+  </si>
+  <si>
+    <t>203.167.214.160</t>
+  </si>
+  <si>
+    <t>59.167.202.57</t>
+  </si>
+  <si>
+    <t>103.22.224.172</t>
+  </si>
+  <si>
+    <t>203.8.4.6</t>
+  </si>
+  <si>
+    <t>43.250.204.36</t>
+  </si>
+  <si>
+    <t>202.125.12.41</t>
+  </si>
+  <si>
+    <t>fqdn</t>
+  </si>
+  <si>
+    <t>10.50.14.132</t>
+  </si>
+  <si>
+    <t>10.50.46.132</t>
+  </si>
+  <si>
+    <t>melairsewer1.dyndns.org</t>
+  </si>
+  <si>
+    <t>peer_id_value</t>
+  </si>
+  <si>
+    <t>esp_authentication</t>
+  </si>
+  <si>
+    <t>esp_encryption</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_IPSEC</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_IPSEC-NEW</t>
+  </si>
+  <si>
+    <t>ADVAM_TEST_IPSEC</t>
+  </si>
+  <si>
+    <t>ADVAM_TEST_IPSEC-NEW</t>
+  </si>
+  <si>
+    <t>AEROCARE_IPSEC</t>
+  </si>
+  <si>
+    <t>AZURE_MEL_IPSEC</t>
+  </si>
+  <si>
+    <t>AZURE_SYD_IPSEC</t>
+  </si>
+  <si>
+    <t>BoM_IPSEC</t>
+  </si>
+  <si>
+    <t>CROSSCOM_IPSEC</t>
+  </si>
+  <si>
+    <t>ESRI_EGIS_IPSEC</t>
+  </si>
+  <si>
+    <t>ETHAN_IPSEC</t>
+  </si>
+  <si>
+    <t>GENTRACK_IPSEC</t>
+  </si>
+  <si>
+    <t>JETSTAR_JINTERNET_IPSec</t>
+  </si>
+  <si>
+    <t>LAUNCESTON_TRANSIT_IPSEC</t>
+  </si>
+  <si>
+    <t>Logicalis_BaaS_IPSEC_Crpto</t>
+  </si>
+  <si>
+    <t>SENSOR_DYNAMICS_IPSEC</t>
+  </si>
+  <si>
+    <t>Verizon_IPSEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> none</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aes-128-gcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aes-256-gcm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no-pfs</t>
   </si>
 </sst>
 </file>
@@ -31056,8 +31374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5A4B3E-AB9B-CE46-94C8-D36C905B2844}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31556,6 +31874,1517 @@
         <v>1440</v>
       </c>
       <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54476EF-3FC4-4248-A28D-878CEA707C75}">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" customWidth="1"/>
+    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2005</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2002</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2003</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2006</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>2008</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>2007</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>2083</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>2009</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>2010</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>985</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>987</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1974</v>
+      </c>
+      <c r="L4" s="2">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>2059</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>2059</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1978</v>
+      </c>
+      <c r="L5" s="2">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>1978</v>
+      </c>
+      <c r="L6" s="2">
+        <v>10</v>
+      </c>
+      <c r="M6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>2061</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>2061</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1979</v>
+      </c>
+      <c r="L7" s="2">
+        <v>10</v>
+      </c>
+      <c r="M7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>2062</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>2062</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="L8" s="2">
+        <v>10</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>1980</v>
+      </c>
+      <c r="L9" s="2">
+        <v>10</v>
+      </c>
+      <c r="M9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>964</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>2041</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>1981</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2021</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2042</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>2065</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2080</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>1983</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>980</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>2043</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>2066</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>2081</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>1984</v>
+      </c>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>2044</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>2067</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>2067</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>2045</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>2068</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>2068</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>2046</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>2069</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>2069</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>1986</v>
+      </c>
+      <c r="L15" s="2">
+        <v>10</v>
+      </c>
+      <c r="M15" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>2047</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>2070</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>2070</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="L16" s="2">
+        <v>10</v>
+      </c>
+      <c r="M16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>2047</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>2071</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>2071</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>1987</v>
+      </c>
+      <c r="L17" s="2">
+        <v>10</v>
+      </c>
+      <c r="M17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>2048</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>2072</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>2072</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>1988</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>2049</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>2073</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>2073</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>1989</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>951</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>2075</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>2075</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>1991</v>
+      </c>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>954</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>2076</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>2076</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>1993</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>2082</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>2079</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>2082</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>2077</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>2077</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>955</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>956</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>2078</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>2004</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>2078</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>2001</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF39C5-BBE3-2C4E-98E2-FCD76E351853}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2084</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2085</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1966</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1968</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>1967</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1973</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>14400</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>2088</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2089</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2090</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2106</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>28800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2091</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1982</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2093</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2106</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>28800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2095</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F13" s="2">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2097</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2106</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2106</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F16" s="2">
+        <v>8</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2100</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1971</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1992</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>1975</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2104</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1997</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2103</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2105</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>2000</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2102</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1976</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>1990</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2">
+        <v>14400</v>
+      </c>
       <c r="H22" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added support to configure IPSec Tunnels and proxyIDs
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sudarshanv/Documents/Projects/panospython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EDA58A-CE9A-FD4D-9F11-75D59D895E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DFDE45-C35A-4743-A617-B521F783E3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="27100" firstSheet="5" activeTab="17" xr2:uid="{D24069A8-A644-D445-BA17-ADF18F8BF45D}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="27100" firstSheet="6" activeTab="19" xr2:uid="{D24069A8-A644-D445-BA17-ADF18F8BF45D}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,8 @@
     <sheet name="ike_crypto_profile" sheetId="16" r:id="rId16"/>
     <sheet name="ike_gateway" sheetId="17" r:id="rId17"/>
     <sheet name="ipsec_crypto_profile" sheetId="18" r:id="rId18"/>
+    <sheet name="ipsec_tunnel" sheetId="19" r:id="rId19"/>
+    <sheet name="ipsec_proxyid" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9420" uniqueCount="2107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9781" uniqueCount="2167">
   <si>
     <t>template_name</t>
   </si>
@@ -6373,6 +6375,186 @@
   </si>
   <si>
     <t xml:space="preserve"> no-pfs</t>
+  </si>
+  <si>
+    <t>pre_shared_key</t>
+  </si>
+  <si>
+    <t>testkey</t>
+  </si>
+  <si>
+    <t>tunnel_interface</t>
+  </si>
+  <si>
+    <t>ak_ipsec_crypto_profile</t>
+  </si>
+  <si>
+    <t>ak_ike_gateway</t>
+  </si>
+  <si>
+    <t>IPSEC-LAUNCESTON-TRANSIT</t>
+  </si>
+  <si>
+    <t>Logicalis_BaaS_MGMT_IPSEC</t>
+  </si>
+  <si>
+    <t>Verizon_vLEC</t>
+  </si>
+  <si>
+    <t>ETHAN_IPSEC_TUNNEL</t>
+  </si>
+  <si>
+    <t>BoM_1_IPSEC_TUNNEL</t>
+  </si>
+  <si>
+    <t>BoM_2_IPSEC_TUNNEL</t>
+  </si>
+  <si>
+    <t>GENTRACK_TUNNEL</t>
+  </si>
+  <si>
+    <t>JETSTAR_JINTERNET_TUNNEL</t>
+  </si>
+  <si>
+    <t>SENSOR_DYNAMICS_TUNNEL</t>
+  </si>
+  <si>
+    <t>ESRI_EGIS_TUNNEL_1</t>
+  </si>
+  <si>
+    <t>ESRI_EGIS_TUNNEL_2</t>
+  </si>
+  <si>
+    <t>AZURE_MEL_TUNNEL</t>
+  </si>
+  <si>
+    <t>AZURE_SYD_TUNNEL</t>
+  </si>
+  <si>
+    <t>SCADA_to_BMS</t>
+  </si>
+  <si>
+    <t>tunnel_name</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>remote</t>
+  </si>
+  <si>
+    <t>Logicalis_BaaS_Proxy</t>
+  </si>
+  <si>
+    <t>Verizon</t>
+  </si>
+  <si>
+    <t>172.26.147.0/27</t>
+  </si>
+  <si>
+    <t>202.125.13.78</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Ethan-1</t>
+  </si>
+  <si>
+    <t>Ethan-2</t>
+  </si>
+  <si>
+    <t>Ethan-3</t>
+  </si>
+  <si>
+    <t>BoM-1</t>
+  </si>
+  <si>
+    <t>172.23.136.0/24</t>
+  </si>
+  <si>
+    <t>BoM-2</t>
+  </si>
+  <si>
+    <t>GENTRACK-1</t>
+  </si>
+  <si>
+    <t>172.24.96.0/27</t>
+  </si>
+  <si>
+    <t>GENTRACK-2</t>
+  </si>
+  <si>
+    <t>GENTRACK-3</t>
+  </si>
+  <si>
+    <t>GENTRACK-4</t>
+  </si>
+  <si>
+    <t>172.25.192.0/22</t>
+  </si>
+  <si>
+    <t>172.23.179.134/32</t>
+  </si>
+  <si>
+    <t>JETSTAR_2</t>
+  </si>
+  <si>
+    <t>RANGE01</t>
+  </si>
+  <si>
+    <t>RANGE02</t>
+  </si>
+  <si>
+    <t>RANGE03</t>
+  </si>
+  <si>
+    <t>RANGE04</t>
+  </si>
+  <si>
+    <t>STAFFtoESRI</t>
+  </si>
+  <si>
+    <t>GENETECtoESRI</t>
+  </si>
+  <si>
+    <t>172.23.21.0/24</t>
+  </si>
+  <si>
+    <t>MAXIMOtoESRI</t>
+  </si>
+  <si>
+    <t>TESTMAXIMOtoESRI</t>
+  </si>
+  <si>
+    <t>SECURITY_DC_TO_ESRP</t>
+  </si>
+  <si>
+    <t>AMStoAZURE</t>
+  </si>
+  <si>
+    <t>10.50.0.0/20</t>
+  </si>
+  <si>
+    <t>CMXtoAZURE</t>
+  </si>
+  <si>
+    <t>FLIRTtoAZURE</t>
+  </si>
+  <si>
+    <t>CENTRALISEDtoAZURE</t>
+  </si>
+  <si>
+    <t>ADVAM_PROD_NEW</t>
+  </si>
+  <si>
+    <t>10.50.32.0/19</t>
+  </si>
+  <si>
+    <t>SewertoBMS</t>
+  </si>
+  <si>
+    <t>any_protocol</t>
   </si>
 </sst>
 </file>
@@ -6467,7 +6649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6487,6 +6669,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31883,10 +32068,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54476EF-3FC4-4248-A28D-878CEA707C75}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31900,12 +32085,13 @@
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -31937,16 +32123,19 @@
         <v>2083</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>2107</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>2009</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>2010</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>2011</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -31978,12 +32167,15 @@
         <v>2056</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>1970</v>
       </c>
-      <c r="L2" s="2"/>
       <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -32015,16 +32207,19 @@
         <v>2057</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>1970</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>10</v>
       </c>
-      <c r="M3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -32056,16 +32251,19 @@
         <v>2058</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>1974</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>10</v>
       </c>
-      <c r="M4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -32097,16 +32295,19 @@
         <v>2059</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>1978</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>10</v>
       </c>
-      <c r="M5" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -32138,16 +32339,19 @@
         <v>2060</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>1978</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>10</v>
       </c>
-      <c r="M6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -32179,16 +32383,19 @@
         <v>2061</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>1979</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>10</v>
       </c>
-      <c r="M7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -32220,16 +32427,19 @@
         <v>2062</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>1980</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>10</v>
       </c>
-      <c r="M8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -32261,16 +32471,19 @@
         <v>2063</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>1980</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>10</v>
       </c>
-      <c r="M9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -32302,12 +32515,15 @@
         <v>2064</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>1981</v>
       </c>
-      <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -32339,12 +32555,15 @@
         <v>2080</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>1983</v>
       </c>
-      <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -32376,12 +32595,15 @@
         <v>2081</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>1984</v>
       </c>
-      <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -32413,12 +32635,15 @@
         <v>2067</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>1985</v>
       </c>
-      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -32450,12 +32675,15 @@
         <v>2068</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>1985</v>
       </c>
-      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -32487,16 +32715,19 @@
         <v>2069</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>1986</v>
-      </c>
-      <c r="L15" s="2">
-        <v>10</v>
       </c>
       <c r="M15" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -32528,16 +32759,19 @@
         <v>2070</v>
       </c>
       <c r="K16" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>1987</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>10</v>
       </c>
-      <c r="M16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -32569,16 +32803,19 @@
         <v>2071</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>1987</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>10</v>
       </c>
-      <c r="M17" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -32610,12 +32847,15 @@
         <v>2072</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>1988</v>
       </c>
-      <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -32647,12 +32887,15 @@
         <v>2073</v>
       </c>
       <c r="K19" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>1989</v>
       </c>
-      <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -32684,12 +32927,15 @@
         <v>2074</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -32721,12 +32967,15 @@
         <v>2075</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>1991</v>
       </c>
-      <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -32758,12 +33007,15 @@
         <v>2076</v>
       </c>
       <c r="K22" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>1993</v>
       </c>
-      <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -32795,12 +33047,15 @@
         <v>2082</v>
       </c>
       <c r="K23" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>1994</v>
       </c>
-      <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -32832,12 +33087,15 @@
         <v>2077</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>1995</v>
       </c>
-      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -32869,10 +33127,13 @@
         <v>2078</v>
       </c>
       <c r="K25" s="2" t="s">
+        <v>2108</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>2001</v>
       </c>
-      <c r="L25" s="2"/>
       <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32883,9 +33144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AF39C5-BBE3-2C4E-98E2-FCD76E351853}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -33386,6 +33645,452 @@
         <v>14400</v>
       </c>
       <c r="H22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8A8C8A-45C8-1447-A5D9-741EBE5B6EC0}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2109</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2111</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2114</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2020</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>2096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2023</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2097</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2014</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>2101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>2122</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2021</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2018</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2019</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>2089</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2016</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1045</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>2022</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>2092</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2013</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>2094</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2025</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>2094</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33544,6 +34249,869 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9589EE7-0B3E-134A-B34B-F531138849AB}">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2166</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2127</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2112</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2113</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2129</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1686</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2114</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2130</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>2131</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2133</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2134</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>2115</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1564</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2116</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2137</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2138</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2139</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>2138</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2140</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2141</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2142</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2143</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2144</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>2146</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>2119</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>2146</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2150</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>1484</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>2120</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2151</v>
+      </c>
+      <c r="D22" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2153</v>
+      </c>
+      <c r="D24" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>2154</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>1547</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1545</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>2121</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2157</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>1559</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>2122</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D28" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2158</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2160</v>
+      </c>
+      <c r="D30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>2123</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>2159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>1615</v>
+      </c>
+      <c r="D34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2163</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2163</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>1624</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>2158</v>
+      </c>
+      <c r="D37" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>1304</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>2160</v>
+      </c>
+      <c r="D38" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>2124</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D41" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>2125</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>2165</v>
+      </c>
+      <c r="D42" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>1433</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>